<commit_message>
Upload author solution for exam preparation II
</commit_message>
<xml_diff>
--- a/Wordpress-Basics/WordPress-Basics-Teachers-September-2018/WordPress-Basics-Teachers-September-2018-Schedule.xlsx
+++ b/Wordpress-Basics/WordPress-Basics-Teachers-September-2018/WordPress-Basics-Teachers-September-2018-Schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>#</t>
   </si>
@@ -40,12 +40,6 @@
     <t>Представяне на задание за проект. Въпроси и отговори.</t>
   </si>
   <si>
-    <t>Професия "Приложен програмист"</t>
-  </si>
-  <si>
-    <t>Какво представлява инициативата на МОН и ИТ асоциациите и как СофтУни помага?</t>
-  </si>
-  <si>
     <t>Урок</t>
   </si>
   <si>
@@ -76,39 +70,18 @@
     <t>Antonia Atanasova</t>
   </si>
   <si>
-    <t>10:00-11:30</t>
-  </si>
-  <si>
     <t>WordPress Basics for Teachers - September 2018</t>
   </si>
   <si>
-    <t>11:30-12:30</t>
-  </si>
-  <si>
-    <t>13:30-15:30</t>
-  </si>
-  <si>
-    <t>Въведение В WordPress</t>
-  </si>
-  <si>
     <t>Работа с WordPress теми</t>
   </si>
   <si>
-    <t>WordPress добавки (PLUGINS)</t>
-  </si>
-  <si>
-    <t>Упражнение: WordPress добавки (PLUGINS)</t>
-  </si>
-  <si>
     <t>Инсталация на WP, създаване на съдържание в WordPress (страници, публикации, мултимедия), хостинг,  домейни.</t>
   </si>
   <si>
     <t>Популярни WP теми, инсталация и настройка на теми.</t>
   </si>
   <si>
-    <t>Полулярни добавки за WP - форми, слайдери, SEO, галерии със снимки, форуми, онлайн магазини и други</t>
-  </si>
-  <si>
     <t>Инсталиране и използване на безплатни WP добавки.</t>
   </si>
   <si>
@@ -118,18 +91,12 @@
     <t>09:30-12:30</t>
   </si>
   <si>
-    <t>14:30-17:30</t>
-  </si>
-  <si>
     <t>Изграждане на WordPress сайт от нулата</t>
   </si>
   <si>
     <t>Създаване на уеб сайт за училище от нулата: инсталиране и настройка на тема, изграждане на начална страница, изграждане на останалите страници.</t>
   </si>
   <si>
-    <t>12:30-13:30</t>
-  </si>
-  <si>
     <t>Представяне на СофтУни</t>
   </si>
   <si>
@@ -137,14 +104,58 @@
   </si>
   <si>
     <t>11:00-18:00</t>
+  </si>
+  <si>
+    <t>10:00-10:30</t>
+  </si>
+  <si>
+    <t>10:30-12:30</t>
+  </si>
+  <si>
+    <t>Упражнение: Въведение в WordPress</t>
+  </si>
+  <si>
+    <t>Въведение в WordPress</t>
+  </si>
+  <si>
+    <t>13:00-15:00</t>
+  </si>
+  <si>
+    <t>Упражнение: Работа с WordPress теми</t>
+  </si>
+  <si>
+    <t>Създаване на уеб сайт в WordPress.com, инсталиране и конфигуриране на WP локално (XAMPP).</t>
+  </si>
+  <si>
+    <t>Инсталиране и персонализиране на безплатна WP тема, импортиране на демо съдържание, промяна на страници.</t>
+  </si>
+  <si>
+    <t>Полулярни добавки за WP - форми, слайдери, SEO, галерии със снимки, форуми, онлайн магазини и други.</t>
+  </si>
+  <si>
+    <t>WordPress добавки (plugins)</t>
+  </si>
+  <si>
+    <t>Упражнение: WordPress добавки (plugins)</t>
+  </si>
+  <si>
+    <t>16:30-17:30</t>
+  </si>
+  <si>
+    <t>09:30-15:30</t>
+  </si>
+  <si>
+    <t>15:30-16:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="d\-mmm"/>
+    <numFmt numFmtId="165" formatCode="dd\-mmm"/>
+    <numFmt numFmtId="166" formatCode="dd/mmm"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -243,9 +254,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -267,14 +275,17 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -708,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="85.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,7 +739,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -742,22 +753,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>13</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -768,151 +779,151 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D3" s="6">
         <v>43371</v>
       </c>
       <c r="E3" s="7" t="str">
-        <f t="shared" ref="E3:E10" si="0">TEXT(D3,"dddd")</f>
+        <f t="shared" ref="E3:E11" si="0">TEXT(D3,"dddd")</f>
         <v>петък</v>
       </c>
-      <c r="F3" s="13" t="s">
-        <v>18</v>
+      <c r="F3" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="12">
+        <v>3</v>
+      </c>
+      <c r="D4" s="11">
         <v>43371</v>
       </c>
-      <c r="E4" s="17" t="str">
-        <f>TEXT(D4,"dddd")</f>
+      <c r="E4" s="7" t="str">
+        <f t="shared" si="0"/>
         <v>петък</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>43371</v>
       </c>
       <c r="E5" s="7" t="str">
         <f t="shared" si="0"/>
         <v>петък</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>4</v>
+      <c r="F5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>1</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>24</v>
+        <v>2</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="12">
+        <v>36</v>
+      </c>
+      <c r="D6" s="11">
         <v>43371</v>
       </c>
-      <c r="E6" s="7" t="str">
-        <f t="shared" si="0"/>
+      <c r="E6" s="16" t="str">
+        <f>TEXT(D6,"dddd")</f>
         <v>петък</v>
       </c>
-      <c r="F6" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>19</v>
+      <c r="F6" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>2</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>25</v>
+        <v>3</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="12">
+        <v>21</v>
+      </c>
+      <c r="D7" s="11">
         <v>43371</v>
       </c>
       <c r="E7" s="7" t="str">
         <f t="shared" si="0"/>
         <v>петък</v>
       </c>
-      <c r="F7" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>19</v>
+      <c r="F7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>3</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>26</v>
+        <v>4</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="8">
+        <v>37</v>
+      </c>
+      <c r="D8" s="16">
         <v>43372</v>
       </c>
-      <c r="E8" s="7" t="str">
-        <f t="shared" si="0"/>
+      <c r="E8" s="19" t="str">
+        <f>TEXT(D8,"dddd")</f>
         <v>събота</v>
       </c>
-      <c r="F8" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>19</v>
+      <c r="F8" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>4</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>31</v>
+        <v>5</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D9" s="8">
         <v>43372</v>
@@ -921,70 +932,70 @@
         <f t="shared" si="0"/>
         <v>събота</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="12" t="s">
-        <v>19</v>
+      <c r="G9" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>5</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>36</v>
+        <v>6</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="D10" s="8">
-        <v>43373</v>
+        <v>43372</v>
       </c>
       <c r="E10" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>неделя</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+        <v>събота</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>6</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="4" t="s">
         <v>7</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="D11" s="8">
         <v>43373</v>
       </c>
-      <c r="E11" s="8" t="str">
-        <f>TEXT(D11,"dddd")</f>
+      <c r="E11" s="7" t="str">
+        <f t="shared" si="0"/>
         <v>неделя</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
+        <v>8</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="D12" s="8">
         <v>43373</v>
@@ -993,45 +1004,58 @@
         <f>TEXT(D12,"dddd")</f>
         <v>неделя</v>
       </c>
-      <c r="F12" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="16">
-        <v>43387</v>
-      </c>
-      <c r="E13" s="17" t="str">
+        <v>15</v>
+      </c>
+      <c r="D13" s="8">
+        <v>43373</v>
+      </c>
+      <c r="E13" s="8" t="str">
         <f>TEXT(D13,"dddd")</f>
         <v>неделя</v>
       </c>
-      <c r="F13" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="10"/>
+      <c r="B14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="15">
+        <v>43387</v>
+      </c>
+      <c r="E14" s="16" t="str">
+        <f>TEXT(D14,"dddd")</f>
+        <v>неделя</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Update schedule for WordPress Basics for Teachers
</commit_message>
<xml_diff>
--- a/Wordpress-Basics/WordPress-Basics-Teachers-September-2018/WordPress-Basics-Teachers-September-2018-Schedule.xlsx
+++ b/Wordpress-Basics/WordPress-Basics-Teachers-September-2018/WordPress-Basics-Teachers-September-2018-Schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t>#</t>
   </si>
@@ -88,9 +88,6 @@
     <t>15:30-17:30</t>
   </si>
   <si>
-    <t>09:30-12:30</t>
-  </si>
-  <si>
     <t>Изграждане на WordPress сайт от нулата</t>
   </si>
   <si>
@@ -109,18 +106,12 @@
     <t>10:00-10:30</t>
   </si>
   <si>
-    <t>10:30-12:30</t>
-  </si>
-  <si>
     <t>Упражнение: Въведение в WordPress</t>
   </si>
   <si>
     <t>Въведение в WordPress</t>
   </si>
   <si>
-    <t>13:00-15:00</t>
-  </si>
-  <si>
     <t>Упражнение: Работа с WordPress теми</t>
   </si>
   <si>
@@ -142,10 +133,22 @@
     <t>16:30-17:30</t>
   </si>
   <si>
-    <t>09:30-15:30</t>
-  </si>
-  <si>
-    <t>15:30-16:00</t>
+    <t>10:30-13:00</t>
+  </si>
+  <si>
+    <t>14:00-16:00</t>
+  </si>
+  <si>
+    <t>16:00-17:30</t>
+  </si>
+  <si>
+    <t>14:00-15:30</t>
+  </si>
+  <si>
+    <t>09:30-13:00</t>
+  </si>
+  <si>
+    <t>16:00-16:30</t>
   </si>
 </sst>
 </file>
@@ -225,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -288,6 +291,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -413,8 +419,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A2:G14" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A2:G14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A2:G15" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A2:G15"/>
   <tableColumns count="7">
     <tableColumn id="1" name="#" dataDxfId="6"/>
     <tableColumn id="2" name="Урок" dataDxfId="5"/>
@@ -717,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="85.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -779,13 +785,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="6">
         <v>43371</v>
       </c>
       <c r="E3" s="7" t="str">
-        <f t="shared" ref="E3:E11" si="0">TEXT(D3,"dddd")</f>
+        <f t="shared" ref="E3:E12" si="0">TEXT(D3,"dddd")</f>
         <v>петък</v>
       </c>
       <c r="F3" s="12" t="s">
@@ -813,7 +819,7 @@
         <v>петък</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>4</v>
@@ -824,7 +830,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>20</v>
@@ -837,7 +843,7 @@
         <v>петък</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>17</v>
@@ -848,10 +854,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D6" s="11">
         <v>43371</v>
@@ -861,7 +867,7 @@
         <v>петък</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>17</v>
@@ -896,10 +902,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D8" s="16">
         <v>43372</v>
@@ -909,7 +915,7 @@
         <v>събота</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>17</v>
@@ -920,10 +926,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D9" s="8">
         <v>43372</v>
@@ -933,7 +939,7 @@
         <v>събота</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>17</v>
@@ -944,7 +950,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>22</v>
@@ -957,7 +963,7 @@
         <v>събота</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>17</v>
@@ -968,58 +974,58 @@
         <v>7</v>
       </c>
       <c r="B11" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="8">
+      <c r="D11" s="16">
         <v>43373</v>
       </c>
-      <c r="E11" s="7" t="str">
+      <c r="E11" s="16" t="str">
         <f t="shared" si="0"/>
         <v>неделя</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>8</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>7</v>
+      <c r="B12" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="D12" s="8">
         <v>43373</v>
       </c>
-      <c r="E12" s="8" t="str">
-        <f>TEXT(D12,"dddd")</f>
+      <c r="E12" s="7" t="str">
+        <f t="shared" si="0"/>
         <v>неделя</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D13" s="8">
         <v>43373</v>
@@ -1028,32 +1034,56 @@
         <f>TEXT(D13,"dddd")</f>
         <v>неделя</v>
       </c>
-      <c r="F13" s="12" t="s">
-        <v>41</v>
+      <c r="F13" s="22" t="s">
+        <v>44</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
+    <row r="14" spans="1:7" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>10</v>
+      </c>
       <c r="B14" s="3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="15">
-        <v>43387</v>
-      </c>
-      <c r="E14" s="16" t="str">
+        <v>15</v>
+      </c>
+      <c r="D14" s="8">
+        <v>43373</v>
+      </c>
+      <c r="E14" s="8" t="str">
         <f>TEXT(D14,"dddd")</f>
         <v>неделя</v>
       </c>
-      <c r="F14" s="17" t="s">
-        <v>29</v>
+      <c r="F14" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="G14" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="15">
+        <v>43387</v>
+      </c>
+      <c r="E15" s="16" t="str">
+        <f>TEXT(D15,"dddd")</f>
+        <v>неделя</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="11" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>